<commit_message>
Added CAN bus pins to chart
</commit_message>
<xml_diff>
--- a/_PinCharts/BBB IO Pins.xlsx
+++ b/_PinCharts/BBB IO Pins.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caibi\Development\2017-18\Shared\Scarlet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Scarlet\_PinCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="63">
   <si>
     <t>Default</t>
   </si>
@@ -205,13 +205,22 @@
   </si>
   <si>
     <t>1_MISO</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>0_RX</t>
+  </si>
+  <si>
+    <t>0_TX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +255,14 @@
       <name val="PT Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="PT Sans"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +335,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9933FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -455,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -595,17 +616,29 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -613,11 +646,8 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,6 +657,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9933FF"/>
+      <color rgb="FF9900FF"/>
+      <color rgb="FF6600CC"/>
       <color rgb="FF33CC33"/>
       <color rgb="FFFFFF66"/>
       <color rgb="FFFF9933"/>
@@ -634,9 +667,6 @@
       <color rgb="FF33CCCC"/>
       <color rgb="FFFF9900"/>
       <color rgb="FFFF6600"/>
-      <color rgb="FF811426"/>
-      <color rgb="FFCC0099"/>
-      <color rgb="FF00FFCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1005,7 +1035,7 @@
   <dimension ref="B2:AB29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,32 +1057,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:28" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
-      <c r="U2" s="50" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="53"/>
+      <c r="U2" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="53"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -1073,10 +1103,10 @@
       <c r="G3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="49"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1109,10 +1139,10 @@
       <c r="W3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="49" t="s">
+      <c r="X3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="49"/>
+      <c r="Y3" s="55"/>
       <c r="Z3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1124,68 +1154,68 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
       <c r="H4" s="10">
         <v>1</v>
       </c>
       <c r="I4" s="11">
         <v>2</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="U4" s="56" t="s">
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="U4" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
       <c r="X4" s="10">
         <v>1</v>
       </c>
       <c r="Y4" s="11">
         <v>2</v>
       </c>
-      <c r="Z4" s="56" t="s">
+      <c r="Z4" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AA4" s="56"/>
-      <c r="AB4" s="56"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="8">
         <v>3</v>
       </c>
       <c r="I5" s="9">
         <v>4</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
       <c r="U5" s="43"/>
       <c r="V5" s="39" t="s">
         <v>16</v>
@@ -1208,28 +1238,28 @@
       <c r="AB5" s="37"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="8">
         <v>5</v>
       </c>
       <c r="I6" s="9">
         <v>6</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
       <c r="U6" s="43"/>
       <c r="V6" s="39" t="s">
         <v>16</v>
@@ -1252,28 +1282,28 @@
       <c r="AB6" s="37"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
       <c r="H7" s="8">
         <v>7</v>
       </c>
       <c r="I7" s="9">
         <v>8</v>
       </c>
-      <c r="J7" s="53" t="s">
+      <c r="J7" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
       <c r="U7" s="43"/>
       <c r="V7" s="39" t="s">
         <v>16</v>
@@ -1296,28 +1326,28 @@
       <c r="AB7" s="37"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
       <c r="H8" s="8">
         <v>9</v>
       </c>
       <c r="I8" s="9">
         <v>10</v>
       </c>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
       <c r="U8" s="43"/>
       <c r="V8" s="39" t="s">
         <v>16</v>
@@ -1551,7 +1581,9 @@
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="C13" s="59" t="s">
+        <v>61</v>
+      </c>
       <c r="D13" s="29" t="s">
         <v>54</v>
       </c>
@@ -1582,7 +1614,9 @@
       <c r="M13" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="N13" s="18"/>
+      <c r="N13" s="50" t="s">
+        <v>62</v>
+      </c>
       <c r="O13" s="18"/>
       <c r="U13" s="44" t="s">
         <v>38</v>
@@ -1700,7 +1734,9 @@
       <c r="M15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="N15" s="48"/>
+      <c r="N15" s="50" t="s">
+        <v>45</v>
+      </c>
       <c r="O15" s="17"/>
       <c r="U15" s="43"/>
       <c r="V15" s="39" t="s">
@@ -1752,7 +1788,9 @@
       <c r="M16" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="48"/>
+      <c r="N16" s="50" t="s">
+        <v>44</v>
+      </c>
       <c r="O16" s="17"/>
       <c r="U16" s="43"/>
       <c r="V16" s="39" t="s">
@@ -1900,14 +1938,14 @@
       <c r="I19" s="9">
         <v>32</v>
       </c>
-      <c r="J19" s="54" t="s">
+      <c r="J19" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
       <c r="U19" s="27"/>
       <c r="V19" s="40" t="s">
         <v>16</v>
@@ -1930,28 +1968,28 @@
       <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
       <c r="H20" s="8">
         <v>33</v>
       </c>
       <c r="I20" s="9">
         <v>34</v>
       </c>
-      <c r="J20" s="54" t="s">
+      <c r="J20" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
       <c r="U20" s="27"/>
       <c r="V20" s="40" t="s">
         <v>16</v>
@@ -1976,28 +2014,28 @@
       </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
       <c r="H21" s="8">
         <v>35</v>
       </c>
       <c r="I21" s="9">
         <v>36</v>
       </c>
-      <c r="J21" s="54" t="s">
+      <c r="J21" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
       <c r="U21" s="27"/>
       <c r="V21" s="40" t="s">
         <v>16</v>
@@ -2022,28 +2060,28 @@
       </c>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="8">
         <v>37</v>
       </c>
       <c r="I22" s="9">
         <v>38</v>
       </c>
-      <c r="J22" s="54" t="s">
+      <c r="J22" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
       <c r="U22" s="27"/>
       <c r="V22" s="40" t="s">
         <v>16</v>
@@ -2066,28 +2104,28 @@
       <c r="AB22" s="13"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="8">
         <v>39</v>
       </c>
       <c r="I23" s="9">
         <v>40</v>
       </c>
-      <c r="J23" s="54" t="s">
+      <c r="J23" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
       <c r="U23" s="27"/>
       <c r="V23" s="40" t="s">
         <v>16</v>
@@ -2162,28 +2200,28 @@
       <c r="AB24" s="13"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
       <c r="H25" s="8">
         <v>43</v>
       </c>
       <c r="I25" s="9">
         <v>44</v>
       </c>
-      <c r="J25" s="53" t="s">
+      <c r="J25" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
       <c r="U25" s="27"/>
       <c r="V25" s="40" t="s">
         <v>16</v>
@@ -2206,28 +2244,28 @@
       <c r="AB25" s="13"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
       <c r="H26" s="8">
         <v>45</v>
       </c>
       <c r="I26" s="9">
         <v>46</v>
       </c>
-      <c r="J26" s="53" t="s">
+      <c r="J26" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
       <c r="U26" s="32" t="s">
         <v>38</v>
       </c>
@@ -2254,36 +2292,47 @@
       </c>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="O29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P29" s="2" t="s">
+      <c r="N29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q29" s="4" t="s">
+      <c r="P29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R29" s="7" t="s">
+      <c r="Q29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S29" s="5" t="s">
+      <c r="R29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T29" s="6" t="s">
+      <c r="S29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="U29" s="55" t="s">
+      <c r="T29" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="U29" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="V29" s="55"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="J19:O19"/>
@@ -2297,18 +2346,11 @@
     <mergeCell ref="J23:O23"/>
     <mergeCell ref="J25:O25"/>
     <mergeCell ref="J26:O26"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="U2:AB2"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="U29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
It's like nothing ever happened to it
</commit_message>
<xml_diff>
--- a/_PinCharts/BBB IO Pins.xlsx
+++ b/_PinCharts/BBB IO Pins.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caibi\Development\Scarlet\_PinCharts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Scarlet\_PinCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24743E91-D281-454A-9637-5F80345008A8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,7 +342,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -473,35 +472,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -578,6 +553,9 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -601,6 +579,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -632,26 +613,32 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -659,49 +646,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1087,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AC29"/>
+  <dimension ref="B2:AB29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,32 +1057,32 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:28" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
-      <c r="U2" s="50" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="53"/>
+      <c r="U2" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="53"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -1158,10 +1103,10 @@
       <c r="G3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="49"/>
+      <c r="I3" s="55"/>
       <c r="J3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1194,10 +1139,10 @@
       <c r="W3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="49" t="s">
+      <c r="X3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="Y3" s="49"/>
+      <c r="Y3" s="55"/>
       <c r="Z3" s="12" t="s">
         <v>30</v>
       </c>
@@ -1209,73 +1154,73 @@
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
       <c r="H4" s="10">
         <v>1</v>
       </c>
       <c r="I4" s="11">
         <v>2</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="U4" s="55" t="s">
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="U4" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="55"/>
-      <c r="W4" s="55"/>
+      <c r="V4" s="54"/>
+      <c r="W4" s="54"/>
       <c r="X4" s="10">
         <v>1</v>
       </c>
       <c r="Y4" s="11">
         <v>2</v>
       </c>
-      <c r="Z4" s="55" t="s">
+      <c r="Z4" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="55"/>
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="8">
         <v>3</v>
       </c>
       <c r="I5" s="9">
         <v>4</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
-      <c r="O5" s="53"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W5" s="30" t="s">
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X5" s="8">
@@ -1284,42 +1229,42 @@
       <c r="Y5" s="9">
         <v>4</v>
       </c>
-      <c r="Z5" s="43" t="s">
+      <c r="Z5" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA5" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB5" s="35"/>
+      <c r="AA5" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB5" s="37"/>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
       <c r="H6" s="8">
         <v>5</v>
       </c>
       <c r="I6" s="9">
         <v>6</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
-      <c r="M6" s="53"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="53"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W6" s="30" t="s">
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W6" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X6" s="8">
@@ -1328,42 +1273,42 @@
       <c r="Y6" s="9">
         <v>6</v>
       </c>
-      <c r="Z6" s="43" t="s">
+      <c r="Z6" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA6" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB6" s="35"/>
+      <c r="AA6" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB6" s="37"/>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
       <c r="H7" s="8">
         <v>7</v>
       </c>
       <c r="I7" s="9">
         <v>8</v>
       </c>
-      <c r="J7" s="53" t="s">
+      <c r="J7" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W7" s="39" t="s">
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X7" s="8">
@@ -1372,42 +1317,42 @@
       <c r="Y7" s="9">
         <v>8</v>
       </c>
-      <c r="Z7" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB7" s="35"/>
+      <c r="Z7" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB7" s="37"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
       <c r="H8" s="8">
         <v>9</v>
       </c>
       <c r="I8" s="9">
         <v>10</v>
       </c>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W8" s="39" t="s">
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
+      <c r="O8" s="57"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W8" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X8" s="8">
@@ -1416,18 +1361,18 @@
       <c r="Y8" s="9">
         <v>10</v>
       </c>
-      <c r="Z8" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB8" s="35"/>
+      <c r="Z8" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB8" s="37"/>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="66"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="23" t="s">
         <v>40</v>
       </c>
@@ -1449,15 +1394,15 @@
       <c r="K9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="57"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="58"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W9" s="39" t="s">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X9" s="8">
@@ -1466,18 +1411,18 @@
       <c r="Y9" s="9">
         <v>12</v>
       </c>
-      <c r="Z9" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB9" s="35"/>
+      <c r="Z9" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB9" s="37"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="67"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="64"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="23" t="s">
         <v>41</v>
       </c>
@@ -1502,16 +1447,16 @@
       <c r="L10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="57"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="58"/>
-      <c r="U10" s="42" t="s">
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="U10" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="V10" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W10" s="39" t="s">
+      <c r="V10" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X10" s="8">
@@ -1520,19 +1465,19 @@
       <c r="Y10" s="9">
         <v>14</v>
       </c>
-      <c r="Z10" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB10" s="35"/>
+      <c r="Z10" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB10" s="37"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="67"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="64"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="24" t="s">
         <v>16</v>
       </c>
@@ -1554,14 +1499,14 @@
       <c r="L11" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="57"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="58"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W11" s="39" t="s">
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W11" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X11" s="8">
@@ -1570,21 +1515,21 @@
       <c r="Y11" s="9">
         <v>16</v>
       </c>
-      <c r="Z11" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB11" s="35"/>
+      <c r="Z11" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB11" s="37"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="68"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="28" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="28" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="24" t="s">
@@ -1611,13 +1556,13 @@
       <c r="M12" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="N12" s="60"/>
-      <c r="O12" s="62"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W12" s="39" t="s">
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X12" s="8">
@@ -1626,23 +1571,23 @@
       <c r="Y12" s="9">
         <v>18</v>
       </c>
-      <c r="Z12" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB12" s="35"/>
+      <c r="Z12" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB12" s="37"/>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="48" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="28" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="24" t="s">
@@ -1669,17 +1614,17 @@
       <c r="M13" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="N13" s="47" t="s">
+      <c r="N13" s="50" t="s">
         <v>62</v>
       </c>
       <c r="O13" s="18"/>
-      <c r="U13" s="42" t="s">
+      <c r="U13" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="V13" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W13" s="39" t="s">
+      <c r="V13" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W13" s="41" t="s">
         <v>0</v>
       </c>
       <c r="X13" s="8">
@@ -1688,25 +1633,25 @@
       <c r="Y13" s="9">
         <v>20</v>
       </c>
-      <c r="Z13" s="43" t="s">
+      <c r="Z13" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA13" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB13" s="35"/>
+      <c r="AA13" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB13" s="37"/>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="28" t="s">
         <v>57</v>
       </c>
       <c r="F14" s="24" t="s">
@@ -1733,17 +1678,17 @@
       <c r="M14" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="N14" s="33" t="s">
+      <c r="N14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="40" t="s">
+      <c r="O14" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="U14" s="41"/>
-      <c r="V14" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W14" s="30" t="s">
+      <c r="U14" s="43"/>
+      <c r="V14" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W14" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X14" s="8">
@@ -1752,19 +1697,19 @@
       <c r="Y14" s="9">
         <v>22</v>
       </c>
-      <c r="Z14" s="43" t="s">
+      <c r="Z14" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA14" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB14" s="35"/>
+      <c r="AA14" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB14" s="37"/>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="67"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="64"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="24" t="s">
         <v>16</v>
       </c>
@@ -1786,18 +1731,18 @@
       <c r="L15" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="M15" s="33" t="s">
+      <c r="M15" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="N15" s="47" t="s">
+      <c r="N15" s="50" t="s">
         <v>45</v>
       </c>
       <c r="O15" s="17"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W15" s="30" t="s">
+      <c r="U15" s="43"/>
+      <c r="V15" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W15" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X15" s="8">
@@ -1806,23 +1751,23 @@
       <c r="Y15" s="9">
         <v>24</v>
       </c>
-      <c r="Z15" s="43" t="s">
+      <c r="Z15" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AA15" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB15" s="35"/>
+      <c r="AA15" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB15" s="37"/>
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="67"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="30" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="31" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="8">
@@ -1840,18 +1785,18 @@
       <c r="L16" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="33" t="s">
+      <c r="M16" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="47" t="s">
+      <c r="N16" s="50" t="s">
         <v>44</v>
       </c>
       <c r="O16" s="17"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="W16" s="30" t="s">
+      <c r="U16" s="43"/>
+      <c r="V16" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="W16" s="31" t="s">
         <v>36</v>
       </c>
       <c r="X16" s="8">
@@ -1860,19 +1805,19 @@
       <c r="Y16" s="9">
         <v>26</v>
       </c>
-      <c r="Z16" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB16" s="35"/>
-    </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B17" s="67"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="64"/>
+      <c r="Z16" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="37"/>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="24" t="s">
         <v>16</v>
       </c>
@@ -1894,14 +1839,14 @@
       <c r="L17" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="M17" s="57"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="58"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W17" s="30" t="s">
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W17" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X17" s="8">
@@ -1910,27 +1855,27 @@
       <c r="Y17" s="9">
         <v>28</v>
       </c>
-      <c r="Z17" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA17" s="44" t="s">
+      <c r="Z17" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA17" s="46" t="s">
         <v>16</v>
       </c>
       <c r="AB17" s="13"/>
     </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B18" s="67"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="27" t="s">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="32" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="31" t="s">
         <v>33</v>
       </c>
       <c r="H18" s="8">
@@ -1948,14 +1893,14 @@
       <c r="L18" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="57"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="58"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W18" s="30" t="s">
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="U18" s="27"/>
+      <c r="V18" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W18" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X18" s="8">
@@ -1964,27 +1909,27 @@
       <c r="Y18" s="9">
         <v>30</v>
       </c>
-      <c r="Z18" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA18" s="44" t="s">
+      <c r="Z18" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA18" s="46" t="s">
         <v>16</v>
       </c>
       <c r="AB18" s="13"/>
     </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B19" s="67"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="27" t="s">
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="32" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="31" t="s">
         <v>33</v>
       </c>
       <c r="H19" s="8">
@@ -1993,19 +1938,19 @@
       <c r="I19" s="9">
         <v>32</v>
       </c>
-      <c r="J19" s="54" t="s">
+      <c r="J19" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
-      <c r="N19" s="54"/>
-      <c r="O19" s="54"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W19" s="30" t="s">
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
+      <c r="U19" s="27"/>
+      <c r="V19" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W19" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X19" s="8">
@@ -2014,42 +1959,42 @@
       <c r="Y19" s="9">
         <v>32</v>
       </c>
-      <c r="Z19" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA19" s="44" t="s">
+      <c r="Z19" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA19" s="46" t="s">
         <v>16</v>
       </c>
       <c r="AB19" s="13"/>
     </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B20" s="54" t="s">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
       <c r="H20" s="8">
         <v>33</v>
       </c>
       <c r="I20" s="9">
         <v>34</v>
       </c>
-      <c r="J20" s="54" t="s">
+      <c r="J20" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54"/>
-      <c r="O20" s="54"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W20" s="30" t="s">
+      <c r="K20" s="58"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="58"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W20" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X20" s="8">
@@ -2058,44 +2003,44 @@
       <c r="Y20" s="9">
         <v>34</v>
       </c>
-      <c r="Z20" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA20" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB20" s="45" t="s">
+      <c r="Z20" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA20" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB20" s="47" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B21" s="54" t="s">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B21" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
       <c r="H21" s="8">
         <v>35</v>
       </c>
       <c r="I21" s="9">
         <v>36</v>
       </c>
-      <c r="J21" s="54" t="s">
+      <c r="J21" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="54"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W21" s="30" t="s">
+      <c r="K21" s="58"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="58"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
+      <c r="U21" s="27"/>
+      <c r="V21" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W21" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X21" s="8">
@@ -2104,44 +2049,44 @@
       <c r="Y21" s="9">
         <v>36</v>
       </c>
-      <c r="Z21" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA21" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB21" s="45" t="s">
+      <c r="Z21" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA21" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB21" s="47" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B22" s="54" t="s">
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B22" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="8">
         <v>37</v>
       </c>
       <c r="I22" s="9">
         <v>38</v>
       </c>
-      <c r="J22" s="54" t="s">
+      <c r="J22" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54"/>
-      <c r="O22" s="54"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W22" s="30" t="s">
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
+      <c r="U22" s="27"/>
+      <c r="V22" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W22" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X22" s="8">
@@ -2150,42 +2095,42 @@
       <c r="Y22" s="9">
         <v>38</v>
       </c>
-      <c r="Z22" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA22" s="44" t="s">
+      <c r="Z22" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA22" s="46" t="s">
         <v>16</v>
       </c>
       <c r="AB22" s="13"/>
     </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B23" s="54" t="s">
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B23" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="8">
         <v>39</v>
       </c>
       <c r="I23" s="9">
         <v>40</v>
       </c>
-      <c r="J23" s="54" t="s">
+      <c r="J23" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="54"/>
-      <c r="O23" s="54"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W23" s="30" t="s">
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W23" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X23" s="8">
@@ -2194,19 +2139,19 @@
       <c r="Y23" s="9">
         <v>40</v>
       </c>
-      <c r="Z23" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA23" s="44" t="s">
+      <c r="Z23" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA23" s="46" t="s">
         <v>16</v>
       </c>
       <c r="AB23" s="13"/>
     </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B24" s="67"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="64"/>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="24" t="s">
         <v>16</v>
       </c>
@@ -2228,16 +2173,16 @@
       <c r="L24" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="M24" s="33" t="s">
+      <c r="M24" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="N24" s="61"/>
-      <c r="O24" s="58"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W24" s="30" t="s">
+      <c r="N24" s="48"/>
+      <c r="O24" s="17"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W24" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X24" s="8">
@@ -2246,42 +2191,42 @@
       <c r="Y24" s="9">
         <v>42</v>
       </c>
-      <c r="Z24" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA24" s="44" t="s">
+      <c r="Z24" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA24" s="46" t="s">
         <v>16</v>
       </c>
       <c r="AB24" s="13"/>
     </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B25" s="53" t="s">
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B25" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
       <c r="H25" s="8">
         <v>43</v>
       </c>
       <c r="I25" s="9">
         <v>44</v>
       </c>
-      <c r="J25" s="53" t="s">
+      <c r="J25" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W25" s="30" t="s">
+      <c r="K25" s="57"/>
+      <c r="L25" s="57"/>
+      <c r="M25" s="57"/>
+      <c r="N25" s="57"/>
+      <c r="O25" s="57"/>
+      <c r="U25" s="27"/>
+      <c r="V25" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W25" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X25" s="8">
@@ -2290,44 +2235,44 @@
       <c r="Y25" s="9">
         <v>44</v>
       </c>
-      <c r="Z25" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA25" s="44" t="s">
+      <c r="Z25" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA25" s="46" t="s">
         <v>16</v>
       </c>
       <c r="AB25" s="13"/>
     </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="s">
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B26" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="57"/>
       <c r="H26" s="8">
         <v>45</v>
       </c>
       <c r="I26" s="9">
         <v>46</v>
       </c>
-      <c r="J26" s="53" t="s">
+      <c r="J26" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="U26" s="31" t="s">
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
+      <c r="M26" s="57"/>
+      <c r="N26" s="57"/>
+      <c r="O26" s="57"/>
+      <c r="U26" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="V26" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="W26" s="30" t="s">
+      <c r="V26" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="W26" s="31" t="s">
         <v>33</v>
       </c>
       <c r="X26" s="8">
@@ -2336,51 +2281,58 @@
       <c r="Y26" s="9">
         <v>46</v>
       </c>
-      <c r="Z26" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA26" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB26" s="45" t="s">
+      <c r="Z26" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA26" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB26" s="47" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
-      <c r="T29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="U29" s="2" t="s">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="N29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V29" s="4" t="s">
+      <c r="P29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="W29" s="7" t="s">
+      <c r="Q29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="X29" s="5" t="s">
+      <c r="R29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Y29" s="6" t="s">
+      <c r="S29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z29" s="46" t="s">
+      <c r="T29" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="AA29" s="56" t="s">
+      <c r="U29" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="AB29" s="56"/>
-      <c r="AC29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="U4:W4"/>
-    <mergeCell ref="Z4:AB4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AA29:AC29"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="J5:O5"/>
+    <mergeCell ref="J6:O6"/>
+    <mergeCell ref="J7:O7"/>
+    <mergeCell ref="J8:O8"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B25:G25"/>
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="J19:O19"/>
@@ -2394,18 +2346,11 @@
     <mergeCell ref="J23:O23"/>
     <mergeCell ref="J25:O25"/>
     <mergeCell ref="J26:O26"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="J5:O5"/>
-    <mergeCell ref="J6:O6"/>
-    <mergeCell ref="J7:O7"/>
-    <mergeCell ref="J8:O8"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="U2:AB2"/>
+    <mergeCell ref="U4:W4"/>
+    <mergeCell ref="Z4:AB4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="U29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>